<commit_message>
Update Pooh Points site
</commit_message>
<xml_diff>
--- a/docs/Today_PoohPoints_SEC_ByOwner_2026-01-07.xlsx
+++ b/docs/Today_PoohPoints_SEC_ByOwner_2026-01-07.xlsx
@@ -540,12 +540,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Nate Ament</t>
+          <t>Tramon Mark</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>TENN</t>
+          <t>TEX</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -559,28 +559,28 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="I2" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="J2" t="n">
         <v>5</v>
       </c>
       <c r="K2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N2" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O2" t="n">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3">
@@ -601,12 +601,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Matas Vokietaitis</t>
+          <t>Nate Ament</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>TEX</t>
+          <t>TENN</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -620,28 +620,28 @@
         </is>
       </c>
       <c r="H3" t="n">
-        <v>-1</v>
+        <v>13</v>
       </c>
       <c r="I3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J3" t="n">
+        <v>5</v>
+      </c>
+      <c r="K3" t="n">
+        <v>2</v>
+      </c>
+      <c r="L3" t="n">
         <v>4</v>
       </c>
-      <c r="J3" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0</v>
-      </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N3" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="O3" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
@@ -657,12 +657,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Tramon Mark</t>
+          <t>Matas Vokietaitis</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -681,28 +681,28 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>19</v>
+        <v>-1</v>
       </c>
       <c r="I4" t="n">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="J4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4" t="n">
         <v>2</v>
       </c>
       <c r="O4" t="n">
-        <v>30</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
@@ -1023,22 +1023,22 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Jacob Crews</t>
+          <t>Billy Richmond III</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>MIZ</t>
+          <t>ARK</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>MIZ@UK</t>
+          <t>ARK@MISS</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -1047,28 +1047,28 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="I10" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="J10" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N10" t="n">
         <v>0</v>
       </c>
       <c r="O10" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11">
@@ -1089,12 +1089,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Billy Richmond III</t>
+          <t>James Scott</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>ARK</t>
+          <t>MISS</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1108,25 +1108,25 @@
         </is>
       </c>
       <c r="H11" t="n">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I11" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="J11" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L11" t="n">
         <v>0</v>
       </c>
       <c r="M11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O11" t="n">
         <v>24</v>
@@ -1150,17 +1150,17 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>James Scott</t>
+          <t>Derrion Reid</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>OU</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>ARK@MISS</t>
+          <t>OU@MSST</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1169,28 +1169,28 @@
         </is>
       </c>
       <c r="H12" t="n">
+        <v>8</v>
+      </c>
+      <c r="I12" t="n">
         <v>11</v>
-      </c>
-      <c r="I12" t="n">
-        <v>6</v>
       </c>
       <c r="J12" t="n">
         <v>3</v>
       </c>
       <c r="K12" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N12" t="n">
         <v>1</v>
       </c>
       <c r="O12" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13">
@@ -1211,17 +1211,17 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Derrion Reid</t>
+          <t>Jacob Crews</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>OU</t>
+          <t>MIZ</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>OU@MSST</t>
+          <t>MIZ@UK</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1230,13 +1230,13 @@
         </is>
       </c>
       <c r="H13" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I13" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="J13" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K13" t="n">
         <v>0</v>
@@ -1245,13 +1245,13 @@
         <v>1</v>
       </c>
       <c r="M13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O13" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14">
@@ -1699,17 +1699,17 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Nijel Pack</t>
+          <t>Meleek Thomas</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>OU</t>
+          <t>ARK</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>OU@MSST</t>
+          <t>ARK@MISS</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1718,28 +1718,28 @@
         </is>
       </c>
       <c r="H21" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I21" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="J21" t="n">
         <v>1</v>
       </c>
       <c r="K21" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L21" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M21" t="n">
         <v>0</v>
       </c>
       <c r="N21" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O21" t="n">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22">
@@ -1882,17 +1882,17 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Meleek Thomas</t>
+          <t>Nijel Pack</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>ARK</t>
+          <t>OU</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>ARK@MISS</t>
+          <t>OU@MSST</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1901,28 +1901,28 @@
         </is>
       </c>
       <c r="H24" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="I24" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J24" t="n">
         <v>1</v>
       </c>
       <c r="K24" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L24" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M24" t="n">
         <v>0</v>
       </c>
       <c r="N24" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O24" t="n">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25">
@@ -2243,22 +2243,22 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Ilias Kamardine</t>
+          <t>Quincy Ballard</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>MISS</t>
+          <t>MSST</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>ARK@MISS</t>
+          <t>OU@MSST</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -2267,28 +2267,28 @@
         </is>
       </c>
       <c r="H30" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="I30" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J30" t="n">
         <v>4</v>
       </c>
       <c r="K30" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L30" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N30" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O30" t="n">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31">
@@ -2309,17 +2309,17 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Quincy Ballard</t>
+          <t>Ilias Kamardine</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>MSST</t>
+          <t>MISS</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>OU@MSST</t>
+          <t>ARK@MISS</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -2328,28 +2328,28 @@
         </is>
       </c>
       <c r="H31" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="I31" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J31" t="n">
         <v>4</v>
       </c>
       <c r="K31" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L31" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N31" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O31" t="n">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32">
@@ -2736,17 +2736,17 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Jaylen Carey</t>
+          <t>Boogie Fland</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>TENN</t>
+          <t>FLA</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>TEX@TENN</t>
+          <t>UGA@FLA</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -2755,28 +2755,28 @@
         </is>
       </c>
       <c r="H38" t="n">
+        <v>12</v>
+      </c>
+      <c r="I38" t="n">
         <v>8</v>
       </c>
-      <c r="I38" t="n">
-        <v>10</v>
-      </c>
       <c r="J38" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="K38" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M38" t="n">
         <v>0</v>
       </c>
       <c r="N38" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O38" t="n">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39">
@@ -2858,17 +2858,17 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Boogie Fland</t>
+          <t>Jaylen Carey</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>FLA</t>
+          <t>TENN</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>UGA@FLA</t>
+          <t>TEX@TENN</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -2877,28 +2877,28 @@
         </is>
       </c>
       <c r="H40" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I40" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J40" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K40" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="L40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M40" t="n">
         <v>0</v>
       </c>
       <c r="N40" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O40" t="n">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41">
@@ -3402,7 +3402,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -3463,22 +3463,22 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Somtochukwu Cyril</t>
+          <t>J.P. Estrella</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>UGA</t>
+          <t>TENN</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>UGA@FLA</t>
+          <t>TEX@TENN</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
@@ -3487,13 +3487,13 @@
         </is>
       </c>
       <c r="H50" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="I50" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="J50" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K50" t="n">
         <v>0</v>
@@ -3502,13 +3502,13 @@
         <v>0</v>
       </c>
       <c r="M50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N50" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O50" t="n">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51">
@@ -3529,17 +3529,17 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>J.P. Estrella</t>
+          <t>Kevin Overton</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>TENN</t>
+          <t>AUB</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>TEX@TENN</t>
+          <t>TA&amp;M@AUB</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -3548,28 +3548,28 @@
         </is>
       </c>
       <c r="H51" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I51" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="J51" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M51" t="n">
         <v>0</v>
       </c>
       <c r="N51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O51" t="n">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="52">
@@ -3590,17 +3590,17 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Kevin Overton</t>
+          <t>Xaivian Lee</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>AUB</t>
+          <t>FLA</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>TA&amp;M@AUB</t>
+          <t>UGA@FLA</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
@@ -3609,28 +3609,28 @@
         </is>
       </c>
       <c r="H52" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I52" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="J52" t="n">
         <v>3</v>
       </c>
       <c r="K52" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L52" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M52" t="n">
         <v>0</v>
       </c>
       <c r="N52" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O52" t="n">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="53">
@@ -3651,12 +3651,12 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Xaivian Lee</t>
+          <t>Somtochukwu Cyril</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>FLA</t>
+          <t>UGA</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -3670,28 +3670,28 @@
         </is>
       </c>
       <c r="H53" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I53" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J53" t="n">
         <v>3</v>
       </c>
       <c r="K53" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L53" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N53" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O53" t="n">
-        <v>27</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54">
@@ -3773,17 +3773,17 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Darius Acuff Jr.</t>
+          <t>Amari Allen</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>ARK</t>
+          <t>ALA</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>ARK@MISS</t>
+          <t>ALA@VAN</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
@@ -3792,28 +3792,28 @@
         </is>
       </c>
       <c r="H55" t="n">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="I55" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J55" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="K55" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="L55" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N55" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O55" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="56">
@@ -3834,17 +3834,17 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Duke Miles</t>
+          <t>Darius Acuff Jr.</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>VAN</t>
+          <t>ARK</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>ALA@VAN</t>
+          <t>ARK@MISS</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
@@ -3853,28 +3853,28 @@
         </is>
       </c>
       <c r="H56" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I56" t="n">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="J56" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K56" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="L56" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N56" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O56" t="n">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="57">
@@ -3895,17 +3895,17 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Xzayvier Brown</t>
+          <t>Duke Miles</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>OU</t>
+          <t>VAN</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>OU@MSST</t>
+          <t>ALA@VAN</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
@@ -3914,28 +3914,28 @@
         </is>
       </c>
       <c r="H57" t="n">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="I57" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="J57" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K57" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L57" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M57" t="n">
         <v>0</v>
       </c>
       <c r="N57" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O57" t="n">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="58">
@@ -3951,22 +3951,22 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Amari Allen</t>
+          <t>Malachi Moreno</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>ALA</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>ALA@VAN</t>
+          <t>MIZ@UK</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
@@ -3975,28 +3975,28 @@
         </is>
       </c>
       <c r="H58" t="n">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="I58" t="n">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="J58" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="K58" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L58" t="n">
         <v>0</v>
       </c>
       <c r="M58" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N58" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O58" t="n">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="59">
@@ -4012,22 +4012,22 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Malachi Moreno</t>
+          <t>Xzayvier Brown</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>OU</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>MIZ@UK</t>
+          <t>OU@MSST</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
@@ -4036,28 +4036,28 @@
         </is>
       </c>
       <c r="H59" t="n">
+        <v>9</v>
+      </c>
+      <c r="I59" t="n">
         <v>13</v>
       </c>
-      <c r="I59" t="n">
-        <v>9</v>
-      </c>
       <c r="J59" t="n">
+        <v>7</v>
+      </c>
+      <c r="K59" t="n">
         <v>4</v>
       </c>
-      <c r="K59" t="n">
-        <v>1</v>
-      </c>
       <c r="L59" t="n">
         <v>0</v>
       </c>
       <c r="M59" t="n">
+        <v>0</v>
+      </c>
+      <c r="N59" t="n">
         <v>3</v>
       </c>
-      <c r="N59" t="n">
-        <v>2</v>
-      </c>
       <c r="O59" t="n">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="60">
@@ -4078,7 +4078,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Blue Cain</t>
+          <t>Marcus Millender</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -4097,28 +4097,28 @@
         </is>
       </c>
       <c r="H60" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="I60" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="J60" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L60" t="n">
         <v>2</v>
       </c>
       <c r="M60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O60" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="61">
@@ -4261,17 +4261,17 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Marcus Millender</t>
+          <t>Rylan Griffen</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>UGA</t>
+          <t>TA&amp;M</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>UGA@FLA</t>
+          <t>TA&amp;M@AUB</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
@@ -4283,25 +4283,25 @@
         <v>18</v>
       </c>
       <c r="I63" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="J63" t="n">
+        <v>6</v>
+      </c>
+      <c r="K63" t="n">
+        <v>1</v>
+      </c>
+      <c r="L63" t="n">
         <v>3</v>
       </c>
-      <c r="K63" t="n">
-        <v>1</v>
-      </c>
-      <c r="L63" t="n">
-        <v>2</v>
-      </c>
       <c r="M63" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O63" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="64">
@@ -4322,17 +4322,17 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Rylan Griffen</t>
+          <t>Blue Cain</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>TA&amp;M</t>
+          <t>UGA</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>TA&amp;M@AUB</t>
+          <t>UGA@FLA</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
@@ -4341,19 +4341,19 @@
         </is>
       </c>
       <c r="H64" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I64" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J64" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K64" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L64" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M64" t="n">
         <v>1</v>
@@ -4362,7 +4362,7 @@
         <v>0</v>
       </c>
       <c r="O64" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="65">
@@ -4505,17 +4505,17 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Mouhamed Dioubate</t>
+          <t>Mohamed Wague</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>OU</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>MIZ@UK</t>
+          <t>OU@MSST</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
@@ -4524,28 +4524,28 @@
         </is>
       </c>
       <c r="H67" t="n">
+        <v>7</v>
+      </c>
+      <c r="I67" t="n">
+        <v>2</v>
+      </c>
+      <c r="J67" t="n">
         <v>5</v>
       </c>
-      <c r="I67" t="n">
-        <v>8</v>
-      </c>
-      <c r="J67" t="n">
-        <v>2</v>
-      </c>
       <c r="K67" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L67" t="n">
         <v>0</v>
       </c>
       <c r="M67" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N67" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O67" t="n">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68">
@@ -4627,17 +4627,17 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Mohamed Wague</t>
+          <t>Mouhamed Dioubate</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>OU</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>OU@MSST</t>
+          <t>MIZ@UK</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
@@ -4646,28 +4646,28 @@
         </is>
       </c>
       <c r="H69" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I69" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J69" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K69" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L69" t="n">
         <v>0</v>
       </c>
       <c r="M69" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N69" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O69" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="70">
@@ -4810,12 +4810,12 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Mike Sharavjamts</t>
+          <t>Max Mackinnon</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>SC</t>
+          <t>LSU</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -4829,28 +4829,28 @@
         </is>
       </c>
       <c r="H72" t="n">
+        <v>7</v>
+      </c>
+      <c r="I72" t="n">
         <v>15</v>
       </c>
-      <c r="I72" t="n">
-        <v>7</v>
-      </c>
       <c r="J72" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="K72" t="n">
+        <v>0</v>
+      </c>
+      <c r="L72" t="n">
+        <v>1</v>
+      </c>
+      <c r="M72" t="n">
+        <v>1</v>
+      </c>
+      <c r="N72" t="n">
         <v>3</v>
       </c>
-      <c r="L72" t="n">
-        <v>1</v>
-      </c>
-      <c r="M72" t="n">
-        <v>2</v>
-      </c>
-      <c r="N72" t="n">
-        <v>0</v>
-      </c>
       <c r="O72" t="n">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="73">
@@ -4932,17 +4932,17 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Elyjah Freeman</t>
+          <t>Mike Sharavjamts</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>AUB</t>
+          <t>SC</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>TA&amp;M@AUB</t>
+          <t>SC@LSU</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
@@ -4951,28 +4951,28 @@
         </is>
       </c>
       <c r="H74" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I74" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J74" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="K74" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L74" t="n">
         <v>1</v>
       </c>
       <c r="M74" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N74" t="n">
         <v>0</v>
       </c>
       <c r="O74" t="n">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
     <row r="75">
@@ -4993,7 +4993,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Tahaad Pettiford</t>
+          <t>Elyjah Freeman</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -5012,28 +5012,28 @@
         </is>
       </c>
       <c r="H75" t="n">
+        <v>10</v>
+      </c>
+      <c r="I75" t="n">
         <v>8</v>
       </c>
-      <c r="I75" t="n">
-        <v>11</v>
-      </c>
       <c r="J75" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N75" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O75" t="n">
-        <v>32</v>
+        <v>15</v>
       </c>
     </row>
     <row r="76">
@@ -5054,17 +5054,17 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Max Mackinnon</t>
+          <t>Tahaad Pettiford</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>LSU</t>
+          <t>AUB</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>SC@LSU</t>
+          <t>TA&amp;M@AUB</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
@@ -5073,28 +5073,28 @@
         </is>
       </c>
       <c r="H76" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I76" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="J76" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K76" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N76" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O76" t="n">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="77">
@@ -5176,17 +5176,17 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Jalen Washington</t>
+          <t>Tae Davis</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>VAN</t>
+          <t>OU</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>ALA@VAN</t>
+          <t>OU@MSST</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
@@ -5195,28 +5195,28 @@
         </is>
       </c>
       <c r="H78" t="n">
+        <v>8</v>
+      </c>
+      <c r="I78" t="n">
+        <v>13</v>
+      </c>
+      <c r="J78" t="n">
         <v>7</v>
       </c>
-      <c r="I78" t="n">
-        <v>9</v>
-      </c>
-      <c r="J78" t="n">
-        <v>3</v>
-      </c>
       <c r="K78" t="n">
         <v>0</v>
       </c>
       <c r="L78" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M78" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N78" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O78" t="n">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="79">
@@ -5359,17 +5359,17 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Tae Davis</t>
+          <t>Jalen Washington</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>OU</t>
+          <t>VAN</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>OU@MSST</t>
+          <t>ALA@VAN</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
@@ -5378,28 +5378,28 @@
         </is>
       </c>
       <c r="H81" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I81" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="J81" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K81" t="n">
         <v>0</v>
       </c>
       <c r="L81" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M81" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N81" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O81" t="n">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="82">
@@ -10086,7 +10086,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="C2" t="n">
         <v>5</v>
@@ -10095,11 +10095,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Hal</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="C3" t="n">
         <v>5</v>
@@ -10108,24 +10108,24 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Clay</t>
+          <t>Hal</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Clay</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="C5" t="n">
         <v>5</v>
@@ -10134,14 +10134,14 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Tar</t>
+          <t>Booz</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -10151,7 +10151,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C7" t="n">
         <v>5</v>
@@ -10160,14 +10160,14 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Booz</t>
+          <t>Tar</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>